<commit_message>
add category and  subcategory changes
add category and  subcategory changes
</commit_message>
<xml_diff>
--- a/uploads/importcategories.xlsx
+++ b/uploads/importcategories.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Commission</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>category Name</t>
   </si>
@@ -359,40 +356,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>